<commit_message>
update. all random rerun (apart from 1st try as initial comparison value)
</commit_message>
<xml_diff>
--- a/Random agents (and learning) performance.xlsx
+++ b/Random agents (and learning) performance.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/caa01c13dfb6bdb4/UZH/Master/19HS/Deep Reinforcement learning/DeepLearning2048/DeepLearning2048/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matte\OneDrive\UZH\Master\19HS\Deep Reinforcement learning\DeepLearning2048\DeepLearning2048\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{28323F50-7491-461B-B34F-993C94DC5856}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{28323F50-7491-461B-B34F-993C94DC5856}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{739217D5-EB4C-4BDF-9D28-39924ABC91E8}"/>
   <bookViews>
     <workbookView xWindow="30720" yWindow="1995" windowWidth="17280" windowHeight="8970" xr2:uid="{18313DEB-2301-465F-AB17-31D94463C195}"/>
   </bookViews>
@@ -48,12 +48,6 @@
     <t>Avg reward</t>
   </si>
   <si>
-    <t>overall training</t>
-  </si>
-  <si>
-    <t>average</t>
-  </si>
-  <si>
     <t>computed</t>
   </si>
   <si>
@@ -63,10 +57,16 @@
     <t>test</t>
   </si>
   <si>
-    <t>random agent</t>
-  </si>
-  <si>
     <t>Tabular Q learning from random agent</t>
+  </si>
+  <si>
+    <t>arithmetic average</t>
+  </si>
+  <si>
+    <t>Test = tabular learning from random agent</t>
+  </si>
+  <si>
+    <t>overall training, 5k episodes</t>
   </si>
 </sst>
 </file>
@@ -418,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80007AED-A9D3-4724-9DF9-1A6CAD427B80}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -429,183 +429,199 @@
     <col min="1" max="1" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="C6">
+        <v>98.43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="C7">
+        <v>90.82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>6.2E-2</v>
+      </c>
+      <c r="C8">
+        <v>98.98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="C9">
+        <v>97.912000000000006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="C10">
+        <v>96.88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="C11">
+        <v>95.26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="C12">
+        <v>95.28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="C13">
+        <v>94.86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>9</v>
+      </c>
+      <c r="B14">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="C14">
+        <v>95.92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="C5">
-        <v>98.43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="C6">
-        <v>90.82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>3</v>
-      </c>
-      <c r="B7">
-        <v>6.2E-2</v>
-      </c>
-      <c r="C7">
-        <v>98.98</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>4</v>
-      </c>
-      <c r="B8">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="C8">
-        <v>97.912000000000006</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>5</v>
-      </c>
-      <c r="B9">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="C9">
-        <v>96.88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>6</v>
-      </c>
-      <c r="B10">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="C10">
-        <v>95.26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>7</v>
-      </c>
-      <c r="B11">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="C11">
-        <v>95.28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>8</v>
-      </c>
-      <c r="B12">
-        <v>4.2000000000000003E-2</v>
-      </c>
-      <c r="C12">
-        <v>94.86</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>9</v>
-      </c>
-      <c r="B13">
-        <v>4.3999999999999997E-2</v>
-      </c>
-      <c r="C13">
-        <v>95.92</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>10</v>
-      </c>
-      <c r="B14">
+      <c r="B15">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <v>90.84</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16">
-        <f>SUM(B5:B14)/10</f>
-        <v>4.4799999999999993E-2</v>
-      </c>
-      <c r="C16">
-        <f>SUM(C5:C14)/10</f>
-        <v>95.518200000000007</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17">
+        <f>SUM(B6:B15)/10</f>
+        <v>4.4799999999999993E-2</v>
+      </c>
+      <c r="C17">
+        <f>SUM(C6:C15)/10</f>
+        <v>95.518200000000007</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>988.66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
+      <c r="E20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
         <v>2</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>3</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="C22">
+        <v>102.71</v>
+      </c>
+      <c r="D22">
+        <v>1219.0899999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>